<commit_message>
c1-resources: update spreadsheet prerequisites
</commit_message>
<xml_diff>
--- a/Course1-Introduction-to-Self-Driving-Cars/resources/Self-Driving-Specialization-Prerequisites-UoT.xlsx
+++ b/Course1-Introduction-to-Self-Driving-Cars/resources/Self-Driving-Specialization-Prerequisites-UoT.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>University of Toronto Self-Driving Specialization Prerequisites</t>
   </si>
@@ -42,6 +42,22 @@
   </si>
   <si>
     <t>Creation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14.0"/>
+      </rPr>
+      <t xml:space="preserve">Github </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Location of this file</t>
+    </r>
   </si>
   <si>
     <r>
@@ -191,12 +207,30 @@
 should be to create a dual boot create a dual-boot to either Linux or Windows 
 in order to setup CARLA </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color rgb="FF1155CC"/>
+        <sz val="16.0"/>
+        <u/>
+      </rPr>
+      <t>Glossary</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16.0"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -232,6 +266,12 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16.0"/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="4">
@@ -658,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -800,6 +840,9 @@
     </xf>
     <xf borderId="27" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1600,11 +1643,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="B20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1657,7 +1702,7 @@
     <row r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -29069,18 +29114,20 @@
       <c r="Z1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="B5:H6"/>
     <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B22"/>
+    <hyperlink r:id="rId1" ref="B20"/>
+    <hyperlink r:id="rId2" ref="B22"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -29102,30 +29149,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -29158,29 +29205,29 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -29204,23 +29251,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -29243,30 +29290,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -29290,13 +29337,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -29311,10 +29358,10 @@
     </row>
     <row r="4">
       <c r="A4" s="43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="37"/>
@@ -29343,10 +29390,10 @@
     </row>
     <row r="5">
       <c r="A5" s="43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="37"/>
@@ -29409,45 +29456,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="48"/>
     </row>
     <row r="3">
       <c r="A3" s="49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="50"/>
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="50"/>
     </row>
     <row r="5">
       <c r="A5" s="49" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="50"/>
     </row>
     <row r="6">
       <c r="A6" s="49" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="50"/>
     </row>
     <row r="7">
       <c r="A7" s="49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="50"/>
     </row>
@@ -29461,16 +29508,16 @@
     </row>
     <row r="10">
       <c r="A10" s="45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="54"/>
     </row>
     <row r="11">
       <c r="A11" s="47" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
@@ -29511,7 +29558,19 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.88"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>